<commit_message>
Added RTX 30 Series Median Pricing Plot
</commit_message>
<xml_diff>
--- a/Spreadsheets/RTX 3060.xlsx
+++ b/Spreadsheets/RTX 3060.xlsx
@@ -481,29 +481,29 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>New ListingNEW NVIDIA GEFORCE RTX 3060-Ti Founders edition (Printed READ DESCRIPTION!!!)</t>
+          <t>New ListingNVIDIA RTX 3060 Ti GIGABYTE EAGLE OC 8GB IN HAND READY TO SHIP</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Brand New · Geforce</t>
+          <t>Brand New · GIGABYTE</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>399.99</v>
+        <v>650</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>10.9</v>
       </c>
       <c r="F2" t="n">
-        <v>399.99</v>
+        <v>660.9</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NEW-NVIDIA-GEFORCE-RTX-3060-Ti-Founders-edition-Printed-READ-DESCRIPTION/402587406466?hash=item5dbc145082:g:unwAAOSwKIBfx~iE</t>
+          <t>https://www.ebay.com/itm/NVIDIA-RTX-3060-Ti-GIGABYTE-EAGLE-OC-8GB-IN-HAND-READY-TO-SHIP/333811666219?hash=item4db8b9cd2b:g:tpEAAOSwbLxfyADU</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>New ListingNvidia Geforce Rtx 3060 Ti Founders Edition (In Hand)</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 TI Founders Edition IN HAND!!!! Limited Stock BUY NOW!!!</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -522,20 +522,20 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>760</v>
+        <v>450</v>
       </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>770</v>
+        <v>450</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/Nvidia-Geforce-Rtx-3060-Ti-Founders-Edition-In-Hand/254796398080?hash=item3b530c7e00:g:zFYAAOSw8XRfx8DI</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-TI-Founders-Edition-IN-HAND-Limited-Stock-BUY-NOW/203206293280?hash=item2f5009f720:g:e7MAAOSwr15fx~hb</t>
         </is>
       </c>
     </row>
@@ -545,7 +545,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>New ListingGeforce RTX 3060 TI Founders Edition ✅ ORDER CONFIRMED ✅</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -554,20 +554,20 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>675</v>
+        <v>399.99</v>
       </c>
       <c r="E4" t="n">
-        <v>51.25</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>726.25</v>
+        <v>399.99</v>
       </c>
       <c r="G4" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/Geforce-RTX-3060-TI-Founders-Edition-ORDER-CONFIRMED/313326580081?hash=item48f3b83171:g:qVYAAOSwNhNfx8FU</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card/313326954368?hash=item48f3bde780:g:~wwAAOSww5hfx9YC</t>
         </is>
       </c>
     </row>
@@ -577,29 +577,29 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 TI Founders Edition IN HAND!!!! Limited Stock BUY NOW!!!</t>
+          <t>New ListingNEW NVIDIA GEFORCE RTX 3060-Ti Founders edition (Printed READ DESCRIPTION!!!)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Brand New · Geforce · 8 GB</t>
+          <t>Brand New · Geforce</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>450</v>
+        <v>399.99</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>450</v>
+        <v>399.99</v>
       </c>
       <c r="G5" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-TI-Founders-Edition-IN-HAND-Limited-Stock-BUY-NOW/203206198312?hash=item2f50088428:g:e7MAAOSwr15fx~hb</t>
+          <t>https://www.ebay.com/itm/NEW-NVIDIA-GEFORCE-RTX-3060-Ti-Founders-edition-Printed-READ-DESCRIPTION/402587406466?hash=item5dbc145082:g:unwAAOSwKIBfx~iE</t>
         </is>
       </c>
     </row>
@@ -609,29 +609,29 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GEFORCE RTX 3060-TI Founders Edition -Printed image file</t>
+          <t>New ListingNvidia Geforce Rtx 3060 Ti Founders Edition (In Hand)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Brand New · Geforce</t>
+          <t>Brand New · Geforce · 8 GB</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>349.99</v>
+        <v>760</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F6" t="n">
-        <v>349.99</v>
+        <v>770</v>
       </c>
       <c r="G6" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GEFORCE-RTX-3060-TI-Founders-Edition-Printed-image-file/174543017549?hash=item28a393164d:g:CiIAAOSwJiBfx~m5</t>
+          <t>https://www.ebay.com/itm/Nvidia-Geforce-Rtx-3060-Ti-Founders-Edition-In-Hand/254796398080?hash=item3b530c7e00:g:zFYAAOSw8XRfx8DI</t>
         </is>
       </c>
     </row>
@@ -641,7 +641,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti Founders Edition Graphics Card - CONFIRMED ORDER</t>
+          <t>New ListingGeforce RTX 3060 TI Founders Edition ✅ ORDER CONFIRMED ✅</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -650,20 +650,20 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>624.99</v>
+        <v>675</v>
       </c>
       <c r="E7" t="n">
-        <v>12</v>
+        <v>51.25</v>
       </c>
       <c r="F7" t="n">
-        <v>636.99</v>
+        <v>726.25</v>
       </c>
       <c r="G7" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-Founders-Edition-Graphics-Card-CONFIRMED-ORDER/124468864150?hash=item1cfaec2496:g:HiQAAOSwb7xfx~PG</t>
+          <t>https://www.ebay.com/itm/Geforce-RTX-3060-TI-Founders-Edition-ORDER-CONFIRMED/313326580081?hash=item48f3b83171:g:qVYAAOSwNhNfx8FU</t>
         </is>
       </c>
     </row>
@@ -673,7 +673,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 TI Founders Edition IN HAND!!!! Limited Stock BUY NOW!!!</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -682,20 +682,20 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>399.99</v>
+        <v>450</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>399.99</v>
+        <v>450</v>
       </c>
       <c r="G8" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card/313326690798?hash=item48f3b9e1ee:g:~wwAAOSww5hfx9YC</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-TI-Founders-Edition-IN-HAND-Limited-Stock-BUY-NOW/203206198312?hash=item2f50088428:g:e7MAAOSwr15fx~hb</t>
         </is>
       </c>
     </row>
@@ -705,29 +705,29 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 TI Founders Edition IN HAND -img</t>
+          <t>New ListingNVIDIA GEFORCE RTX 3060-TI Founders Edition -Printed image file</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Brand New · NVIDIA · NVIDIA GeForce RTX 2080 Ti · 11GB</t>
+          <t>Brand New · Geforce</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>399.99</v>
+        <v>349.99</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>399.99</v>
+        <v>349.99</v>
       </c>
       <c r="G9" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-TI-Founders-Edition-IN-HAND-img/254796573706?epid=9026714548&amp;hash=item3b530f2c0a:g:HP0AAOSwbAlfx-I4</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GEFORCE-RTX-3060-TI-Founders-Edition-Printed-image-file/174543017549?hash=item28a393164d:g:CiIAAOSwJiBfx~m5</t>
         </is>
       </c>
     </row>
@@ -737,29 +737,29 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GEFORCE RTX 3060 Ti ASUS TUF BRAND NEW Shipping Same Day</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti Founders Edition Graphics Card - CONFIRMED ORDER</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Brand New · ASUS</t>
+          <t>Brand New · Geforce · 8 GB</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>680</v>
+        <v>624.99</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F10" t="n">
-        <v>680</v>
+        <v>636.99</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GEFORCE-RTX-3060-Ti-ASUS-TUF-BRAND-NEW-Shipping-Same-Day/184563131594?hash=item2af8d1e4ca:g:u1EAAOSwSadfx-Yb</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-Founders-Edition-Graphics-Card-CONFIRMED-ORDER/124468864150?hash=item1cfaec2496:g:HiQAAOSwb7xfx~PG</t>
         </is>
       </c>
     </row>
@@ -769,7 +769,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card  *PRE ORDER*</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -778,20 +778,20 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>600</v>
+        <v>399.99</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>600</v>
+        <v>399.99</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card-PRE-ORDER/203206000342?hash=item2f50057ed6:g:ok4AAOSwhtpfx8V0</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card/313326690798?hash=item48f3b9e1ee:g:~wwAAOSww5hfx9YC</t>
         </is>
       </c>
     </row>
@@ -801,29 +801,29 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>New ListingMSI RTX 3060 TI VENTUS 2x OC</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 TI Founders Edition IN HAND -img</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Brand New · MSI</t>
+          <t>Brand New · NVIDIA · NVIDIA GeForce RTX 2080 Ti · 11GB</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>749.99</v>
+        <v>399.99</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>749.99</v>
+        <v>399.99</v>
       </c>
       <c r="G12" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/MSI-RTX-3060-TI-VENTUS-2x-OC/293870587725?hash=item446c0d4f4d:g:GsUAAOSwzqtfx7zL</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-TI-Founders-Edition-IN-HAND-img/254796573706?epid=9026714548&amp;hash=item3b530f2c0a:g:HP0AAOSwbAlfx-I4</t>
         </is>
       </c>
     </row>
@@ -833,29 +833,29 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GEFORCE RTX 3060-TI Founders Edition -Printed image file</t>
+          <t>New ListingNVIDIA GEFORCE RTX 3060 Ti ASUS TUF BRAND NEW Shipping Same Day</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Brand New · Geforce</t>
+          <t>Brand New · ASUS</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>350</v>
+        <v>680</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>350</v>
+        <v>680</v>
       </c>
       <c r="G13" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GEFORCE-RTX-3060-TI-Founders-Edition-Printed-image-file/114554126415?hash=item1aabf5404f:g:B2gAAOSw4h1fx8jO</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GEFORCE-RTX-3060-Ti-ASUS-TUF-BRAND-NEW-Shipping-Same-Day/184563131594?hash=item2af8d1e4ca:g:u1EAAOSwSadfx-Yb</t>
         </is>
       </c>
     </row>
@@ -865,29 +865,29 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>New ListingZOTAC GAMING GeForce RTX 3060 Ti Twin Edge  ZT-A30610E-10M - Confirmed Order</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card  *PRE ORDER*</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Brand New · ZOTAC · 8 GB</t>
+          <t>Brand New · Geforce · 8 GB</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>650</v>
+        <v>600</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>650</v>
+        <v>600</v>
       </c>
       <c r="G14" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/ZOTAC-GAMING-GeForce-RTX-3060-Ti-Twin-Edge-ZT-A30610E-10M-Confirmed-Order/124468762281?hash=item1cfaea96a9:g:IyoAAOSw-JRfx9Dx</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card-PRE-ORDER/203206000342?hash=item2f50057ed6:g:ok4AAOSwhtpfx8V0</t>
         </is>
       </c>
     </row>
@@ -897,29 +897,29 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>New ListingNvidia Geforce RTX 3060 TI Founders Edition Graphics Card</t>
+          <t>New ListingMSI RTX 3060 TI VENTUS 2x OC</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Brand New · Geforce · 8 GB</t>
+          <t>Brand New · MSI</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>799.99</v>
+        <v>749.99</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>799.99</v>
+        <v>749.99</v>
       </c>
       <c r="G15" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/Nvidia-Geforce-RTX-3060-TI-Founders-Edition-Graphics-Card/154223534375?hash=item23e8706127:g:sNcAAOSw7Hlfx7M-</t>
+          <t>https://www.ebay.com/itm/MSI-RTX-3060-TI-VENTUS-2x-OC/293870587725?hash=item446c0d4f4d:g:GsUAAOSwzqtfx7zL</t>
         </is>
       </c>
     </row>
@@ -929,29 +929,29 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6 PCI Express 4.0 Graphics Card order confirm</t>
+          <t>New ListingNVIDIA GEFORCE RTX 3060-TI Founders Edition -Printed image file</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Brand New · Nvida · 8 GB</t>
+          <t>Brand New · Geforce</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>699</v>
+        <v>350</v>
       </c>
       <c r="E16" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>708</v>
+        <v>350</v>
       </c>
       <c r="G16" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6-PCI-Express-4-0-Graphics-Card-order-confirm/114554114008?hash=item1aabf50fd8:g:SnkAAOSwSBpfx7Zr</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GEFORCE-RTX-3060-TI-Founders-Edition-Printed-image-file/114554126415?hash=item1aabf5404f:g:B2gAAOSw4h1fx8jO</t>
         </is>
       </c>
     </row>
@@ -961,12 +961,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card  *SHIPS 12/9*</t>
+          <t>New ListingZOTAC GAMING GeForce RTX 3060 Ti Twin Edge  ZT-A30610E-10M - Confirmed Order</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Brand New · Geforce · 8 GB</t>
+          <t>Brand New · ZOTAC · 8 GB</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -983,7 +983,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card-SHIPS-12-9/164553091737?hash=item265020ea99:g:f0YAAOSwyHhfx75S</t>
+          <t>https://www.ebay.com/itm/ZOTAC-GAMING-GeForce-RTX-3060-Ti-Twin-Edge-ZT-A30610E-10M-Confirmed-Order/124468762281?hash=item1cfaea96a9:g:IyoAAOSw-JRfx9Dx</t>
         </is>
       </c>
     </row>
@@ -993,29 +993,29 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>New ListingMSI - Geforce RTX 3060 Ti VENTUS 2X IN HAND &amp; SHIPS TODAY</t>
+          <t>New ListingNvidia Geforce RTX 3060 TI Founders Edition Graphics Card</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Brand New · MSI · 8 GB</t>
+          <t>Brand New · Geforce · 8 GB</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>649.99</v>
+        <v>799.99</v>
       </c>
       <c r="E18" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>664.99</v>
+        <v>799.99</v>
       </c>
       <c r="G18" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/MSI-Geforce-RTX-3060-Ti-VENTUS-2X-IN-HAND-SHIPS-TODAY/284101619107?hash=item4225c6ada3:g:ZhMAAOSwhkdfx9-w</t>
+          <t>https://www.ebay.com/itm/Nvidia-Geforce-RTX-3060-TI-Founders-Edition-Graphics-Card/154223534375?hash=item23e8706127:g:sNcAAOSw7Hlfx7M-</t>
         </is>
       </c>
     </row>
@@ -1034,20 +1034,20 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>675</v>
+        <v>699</v>
       </c>
       <c r="E19" t="n">
-        <v>15.05</v>
+        <v>9</v>
       </c>
       <c r="F19" t="n">
-        <v>690.05</v>
+        <v>708</v>
       </c>
       <c r="G19" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6-PCI-Express-4-0-Graphics-Card-order-confirm/264961448575?hash=item3db0eeda7f:g:ql0AAOSwsfpfx83q</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6-PCI-Express-4-0-Graphics-Card-order-confirm/114554114008?hash=item1aabf50fd8:g:SnkAAOSwSBpfx7Zr</t>
         </is>
       </c>
     </row>
@@ -1057,7 +1057,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card Confirmed!</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card  *SHIPS 12/9*</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1066,20 +1066,20 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>670</v>
+        <v>650</v>
       </c>
       <c r="E20" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>675</v>
+        <v>650</v>
       </c>
       <c r="G20" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card-Confirmed/184562900094?hash=item2af8ce5c7e:g:sZgAAOSwTC5fx7g3</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card-SHIPS-12-9/164553091737?hash=item265020ea99:g:f0YAAOSwyHhfx75S</t>
         </is>
       </c>
     </row>
@@ -1089,29 +1089,29 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card</t>
+          <t>New ListingMSI - Geforce RTX 3060 Ti VENTUS 2X IN HAND &amp; SHIPS TODAY</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Brand New · Geforce · 8 GB</t>
+          <t>Brand New · MSI · 8 GB</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>600</v>
+        <v>649.99</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F21" t="n">
-        <v>600</v>
+        <v>664.99</v>
       </c>
       <c r="G21" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card/124468523513?hash=item1cfae6f1f9:g:QasAAOSwdhNfx8q1</t>
+          <t>https://www.ebay.com/itm/MSI-Geforce-RTX-3060-Ti-VENTUS-2X-IN-HAND-SHIPS-TODAY/284101619107?hash=item4225c6ada3:g:ZhMAAOSwhkdfx9-w</t>
         </is>
       </c>
     </row>
@@ -1121,29 +1121,29 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>New ListingNvidia GeForce RTX 3060 Ti Founders Edition *IN HAND* FAST SHIPPING</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6 PCI Express 4.0 Graphics Card order confirm</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Brand New · Geforce · 8 GB</t>
+          <t>Brand New · Nvida · 8 GB</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>749.99</v>
+        <v>675</v>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>15.05</v>
       </c>
       <c r="F22" t="n">
-        <v>749.99</v>
+        <v>690.05</v>
       </c>
       <c r="G22" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/Nvidia-GeForce-RTX-3060-Ti-Founders-Edition-IN-HAND-FAST-SHIPPING/284101636291?hash=item4225c6f0c3:g:rwoAAOSwfw5fx9hT</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6-PCI-Express-4-0-Graphics-Card-order-confirm/264961448575?hash=item3db0eeda7f:g:ql0AAOSwsfpfx83q</t>
         </is>
       </c>
     </row>
@@ -1153,7 +1153,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6 PCI Express 4.0 - Steel and Black Preorder</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card Confirmed!</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1162,20 +1162,20 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>649</v>
+        <v>670</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F23" t="n">
-        <v>649</v>
+        <v>675</v>
       </c>
       <c r="G23" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6-PCI-Express-4-0-Steel-and-Black-Preorder/363204598878?hash=item5490ae5c5e:g:fwsAAOSwViVfx8bf</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card-Confirmed/184562900094?hash=item2af8ce5c7e:g:sZgAAOSwTC5fx7g3</t>
         </is>
       </c>
     </row>
@@ -1185,7 +1185,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>New ListingNvidia GeForce RTX 3060 Ti Founders Edition *IN HAND* FAST SHIPPING</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1194,20 +1194,20 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>749.99</v>
+        <v>600</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>749.99</v>
+        <v>600</v>
       </c>
       <c r="G24" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/Nvidia-GeForce-RTX-3060-Ti-Founders-Edition-IN-HAND-FAST-SHIPPING/284101583429?hash=item4225c62245:g:rwoAAOSwfw5fx9hT</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card/124468523513?hash=item1cfae6f1f9:g:QasAAOSwdhNfx8q1</t>
         </is>
       </c>
     </row>
@@ -1217,29 +1217,29 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>New ListingNvidia GeForce RTX 3060 ti Founders Edition (picture)</t>
+          <t>New ListingNvidia GeForce RTX 3060 Ti Founders Edition *IN HAND* FAST SHIPPING</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Brand New · NVIDIA</t>
+          <t>Brand New · Geforce · 8 GB</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>399</v>
+        <v>749.99</v>
       </c>
       <c r="E25" t="n">
-        <v>16.9</v>
+        <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>415.9</v>
+        <v>749.99</v>
       </c>
       <c r="G25" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/Nvidia-GeForce-RTX-3060-ti-Founders-Edition-picture/184563106305?hash=item2af8d18201:g:juQAAOSwdtxfx82G</t>
+          <t>https://www.ebay.com/itm/Nvidia-GeForce-RTX-3060-Ti-Founders-Edition-IN-HAND-FAST-SHIPPING/284101636291?hash=item4225c6f0c3:g:rwoAAOSwfw5fx9hT</t>
         </is>
       </c>
     </row>
@@ -1249,29 +1249,29 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6 PCI Graphics Card Founders Edition IN-HAND</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6 PCI Express 4.0 - Steel and Black Preorder</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Brand New · Nvida · 8 GB</t>
+          <t>Brand New · Geforce · 8 GB</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>699.99</v>
+        <v>649</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>699.99</v>
+        <v>649</v>
       </c>
       <c r="G26" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6-PCI-Graphics-Card-Founders-Edition-IN-HAND/124468701687?hash=item1cfae9a9f7:g:taAAAOSwlAdfx93c</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6-PCI-Express-4-0-Steel-and-Black-Preorder/363204598878?hash=item5490ae5c5e:g:fwsAAOSwViVfx8bf</t>
         </is>
       </c>
     </row>
@@ -1281,7 +1281,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA Geforce RTX 3060-TI Founders Edition Image In Hand</t>
+          <t>New ListingNvidia GeForce RTX 3060 Ti Founders Edition *IN HAND* FAST SHIPPING</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1290,20 +1290,20 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>399.99</v>
+        <v>749.99</v>
       </c>
       <c r="E27" t="n">
         <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>399.99</v>
+        <v>749.99</v>
       </c>
       <c r="G27" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-Geforce-RTX-3060-TI-Founders-Edition-Image-In-Hand/313326703974?hash=item48f3ba1566:g:X7kAAOSwzHdfx9js</t>
+          <t>https://www.ebay.com/itm/Nvidia-GeForce-RTX-3060-Ti-Founders-Edition-IN-HAND-FAST-SHIPPING/284101583429?hash=item4225c62245:g:rwoAAOSwfw5fx9hT</t>
         </is>
       </c>
     </row>
@@ -1313,29 +1313,29 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB Founder's Edition</t>
+          <t>New ListingNvidia GeForce RTX 3060 ti Founders Edition (picture)</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Brand New · NVIDIA · 8 GB</t>
+          <t>Brand New · NVIDIA</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>649.99</v>
+        <v>399</v>
       </c>
       <c r="E28" t="n">
-        <v>0</v>
+        <v>16.9</v>
       </c>
       <c r="F28" t="n">
-        <v>649.99</v>
+        <v>415.9</v>
       </c>
       <c r="G28" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-Founders-Edition/264961475060?hash=item3db0ef41f4:g:cUIAAOSwbVVfx7sA</t>
+          <t>https://www.ebay.com/itm/Nvidia-GeForce-RTX-3060-ti-Founders-Edition-picture/184563106305?hash=item2af8d18201:g:juQAAOSwdtxfx82G</t>
         </is>
       </c>
     </row>
@@ -1345,29 +1345,29 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>New ListingRTX 3060 TI Founders Edition * IN HAND *</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6 PCI Graphics Card Founders Edition IN-HAND</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Brand New · Geforce · 8 GB</t>
+          <t>Brand New · Nvida · 8 GB</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>639.99</v>
+        <v>699.99</v>
       </c>
       <c r="E29" t="n">
-        <v>8.699999999999999</v>
+        <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>648.6900000000001</v>
+        <v>699.99</v>
       </c>
       <c r="G29" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/RTX-3060-TI-Founders-Edition-IN-HAND/324401933064?hash=item4b87dcab08:g:Hq8AAOSwuqNfx9Xi</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6-PCI-Graphics-Card-Founders-Edition-IN-HAND/124468701687?hash=item1cfae9a9f7:g:taAAAOSwlAdfx93c</t>
         </is>
       </c>
     </row>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>New ListingNEW NVIDIA GEFORCE RTX 3060-TI FOUNDERS EDITION-img file</t>
+          <t>New ListingNVIDIA Geforce RTX 3060-TI Founders Edition Image In Hand</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1386,20 +1386,20 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>410</v>
+        <v>399.99</v>
       </c>
       <c r="E30" t="n">
         <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>410</v>
+        <v>399.99</v>
       </c>
       <c r="G30" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NEW-NVIDIA-GEFORCE-RTX-3060-TI-FOUNDERS-EDITION-img-file/303792360445?hash=item46bb6f8bfd:g:If4AAOSwKcxfx3J8</t>
+          <t>https://www.ebay.com/itm/NVIDIA-Geforce-RTX-3060-TI-Founders-Edition-Image-In-Hand/313326703974?hash=item48f3ba1566:g:X7kAAOSwzHdfx9js</t>
         </is>
       </c>
     </row>
@@ -1409,29 +1409,29 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6 PCI Graphics Card IN-HAND SHIPS TODAY</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB Founder's Edition</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Brand New · Nvida · 8 GB</t>
+          <t>Brand New · NVIDIA · 8 GB</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>699.99</v>
+        <v>649.99</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>699.99</v>
+        <v>649.99</v>
       </c>
       <c r="G31" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6-PCI-Graphics-Card-IN-HAND-SHIPS-TODAY/324401859560?hash=item4b87db8be8:g:Ep0AAOSwpE5fx8le</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-Founders-Edition/264961475060?hash=item3db0ef41f4:g:cUIAAOSwbVVfx7sA</t>
         </is>
       </c>
     </row>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t xml:space="preserve">New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card  *PRE ORDER* </t>
+          <t>New ListingRTX 3060 TI Founders Edition * IN HAND *</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1450,20 +1450,20 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>649.95</v>
+        <v>639.99</v>
       </c>
       <c r="E32" t="n">
-        <v>10.95</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="F32" t="n">
-        <v>660.9000000000001</v>
+        <v>648.6900000000001</v>
       </c>
       <c r="G32" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card-PRE-ORDER/193776692074?hash=item2d1dfdab6a:g:4MYAAOSwjN5fx8Ps</t>
+          <t>https://www.ebay.com/itm/RTX-3060-TI-Founders-Edition-IN-HAND/324401933064?hash=item4b87dcab08:g:Hq8AAOSwuqNfx9Xi</t>
         </is>
       </c>
     </row>
@@ -1473,7 +1473,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card  *PRE ORDER*</t>
+          <t>New ListingNEW NVIDIA GEFORCE RTX 3060-TI FOUNDERS EDITION-img file</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1482,20 +1482,20 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>649.99</v>
+        <v>410</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>649.99</v>
+        <v>410</v>
       </c>
       <c r="G33" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card-PRE-ORDER/133594861719?hash=item1f1adfd097:g:rTcAAOSwCH9fx7SO</t>
+          <t>https://www.ebay.com/itm/NEW-NVIDIA-GEFORCE-RTX-3060-TI-FOUNDERS-EDITION-img-file/303792360445?hash=item46bb6f8bfd:g:If4AAOSwKcxfx3J8</t>
         </is>
       </c>
     </row>
@@ -1505,29 +1505,29 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 TI Founders Edition (picture) for robots</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6 PCI Graphics Card IN-HAND SHIPS TODAY</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Brand New · NVIDIA · NVIDIA GeForce RTX 2080 Ti · 11GB</t>
+          <t>Brand New · Nvida · 8 GB</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>419</v>
+        <v>699.99</v>
       </c>
       <c r="E34" t="n">
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>419</v>
+        <v>699.99</v>
       </c>
       <c r="G34" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-TI-Founders-Edition-picture-for-robots/233805488041?epid=9026714548&amp;hash=item366fe49fa9:g:V4UAAOSwvrFfx6aj</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6-PCI-Graphics-Card-IN-HAND-SHIPS-TODAY/324401859560?hash=item4b87db8be8:g:Ep0AAOSwpE5fx8le</t>
         </is>
       </c>
     </row>
@@ -1537,29 +1537,29 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>New ListingAsus Tuf Geforce RTX 3060 Ti OC 8GB</t>
+          <t xml:space="preserve">New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card  *PRE ORDER* </t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Brand New · ASUS · 8 GB</t>
+          <t>Brand New · Geforce · 8 GB</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>649.99</v>
+        <v>649.95</v>
       </c>
       <c r="E35" t="n">
-        <v>11.55</v>
+        <v>10.95</v>
       </c>
       <c r="F35" t="n">
-        <v>661.54</v>
+        <v>660.9000000000001</v>
       </c>
       <c r="G35" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/Asus-Tuf-Geforce-RTX-3060-Ti-OC-8GB/143869920440?hash=item217f50c4b8:g:VEgAAOSwsHhfx8g6</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card-PRE-ORDER/193776692074?hash=item2d1dfdab6a:g:4MYAAOSwjN5fx8Ps</t>
         </is>
       </c>
     </row>
@@ -1569,29 +1569,29 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>New ListingZOTAC GAMING GeForce RTX 3060 Ti Twin Edge OC - ZT-A30610H-10M - Confirmed Order</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card  *PRE ORDER*</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Brand New · ZOTAC · 8 GB</t>
+          <t>Brand New · Geforce · 8 GB</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>650</v>
+        <v>649.99</v>
       </c>
       <c r="E36" t="n">
         <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>650</v>
+        <v>649.99</v>
       </c>
       <c r="G36" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/ZOTAC-GAMING-GeForce-RTX-3060-Ti-Twin-Edge-OC-ZT-A30610H-10M-Confirmed-Order/174542801969?hash=item28a38fcc31:g:edkAAOSw9-9fx70Z</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card-PRE-ORDER/133594861719?hash=item1f1adfd097:g:rTcAAOSwCH9fx7SO</t>
         </is>
       </c>
     </row>
@@ -1601,29 +1601,29 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>New ListingNvidia GeForce RTX 3060 ti Founders Edition</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 TI Founders Edition (picture) for robots</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Brand New · NVIDIA</t>
+          <t>Brand New · NVIDIA · NVIDIA GeForce RTX 2080 Ti · 11GB</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>399</v>
+        <v>419</v>
       </c>
       <c r="E37" t="n">
-        <v>16.9</v>
+        <v>0</v>
       </c>
       <c r="F37" t="n">
-        <v>415.9</v>
+        <v>419</v>
       </c>
       <c r="G37" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/Nvidia-GeForce-RTX-3060-ti-Founders-Edition/184563000100?hash=item2af8cfe324:g:juQAAOSwdtxfx82G</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-TI-Founders-Edition-picture-for-robots/233805488041?epid=9026714548&amp;hash=item366fe49fa9:g:V4UAAOSwvrFfx6aj</t>
         </is>
       </c>
     </row>
@@ -1633,29 +1633,29 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>New ListingEVGA GeForce RTX 3060 Ti FTW3 ULTRA GAMING Ready to ship!</t>
+          <t>New ListingAsus Tuf Geforce RTX 3060 Ti OC 8GB</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Brand New · NVIDIA · 8 GB</t>
+          <t>Brand New · ASUS · 8 GB</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>700</v>
+        <v>649.99</v>
       </c>
       <c r="E38" t="n">
-        <v>0</v>
+        <v>11.55</v>
       </c>
       <c r="F38" t="n">
-        <v>700</v>
+        <v>661.54</v>
       </c>
       <c r="G38" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/EVGA-GeForce-RTX-3060-Ti-FTW3-ULTRA-GAMING-Ready-to-ship/264961477720?hash=item3db0ef4c58:g:zhcAAOSwxVFfx8th</t>
+          <t>https://www.ebay.com/itm/Asus-Tuf-Geforce-RTX-3060-Ti-OC-8GB/143869920440?hash=item217f50c4b8:g:VEgAAOSwsHhfx8g6</t>
         </is>
       </c>
     </row>
@@ -1665,29 +1665,29 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6 PCI Express 4.0 Graphics Card *img*</t>
+          <t>New ListingZOTAC GAMING GeForce RTX 3060 Ti Twin Edge OC - ZT-A30610H-10M - Confirmed Order</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Brand New · Geforce · 8 GB</t>
+          <t>Brand New · ZOTAC · 8 GB</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>500</v>
+        <v>650</v>
       </c>
       <c r="E39" t="n">
-        <v>3.8</v>
+        <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>503.8</v>
+        <v>650</v>
       </c>
       <c r="G39" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6-PCI-Express-4-0-Graphics-Card-img/393040327541?hash=item5b83077375:g:oIUAAOSwi3Bfx7gu</t>
+          <t>https://www.ebay.com/itm/ZOTAC-GAMING-GeForce-RTX-3060-Ti-Twin-Edge-OC-ZT-A30610H-10M-Confirmed-Order/174542801969?hash=item28a38fcc31:g:edkAAOSw9-9fx70Z</t>
         </is>
       </c>
     </row>
@@ -1697,29 +1697,29 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card</t>
+          <t>New ListingNvidia GeForce RTX 3060 ti Founders Edition</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Brand New · Geforce · 8 GB</t>
+          <t>Brand New · NVIDIA</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>650</v>
+        <v>399</v>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
+        <v>16.9</v>
       </c>
       <c r="F40" t="n">
-        <v>650</v>
+        <v>415.9</v>
       </c>
       <c r="G40" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card/264961483895?hash=item3db0ef6477:g:kdoAAOSw2PVfx7MO</t>
+          <t>https://www.ebay.com/itm/Nvidia-GeForce-RTX-3060-ti-Founders-Edition/184563000100?hash=item2af8cfe324:g:juQAAOSwdtxfx82G</t>
         </is>
       </c>
     </row>
@@ -1729,29 +1729,29 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6 PCI Express 4.0 Graphics Card *PREORDER*</t>
+          <t>New ListingEVGA GeForce RTX 3060 Ti FTW3 ULTRA GAMING Ready to ship!</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>*PRE-ORDER! SHIPS OUT ON DECEMBER 8</t>
+          <t>Brand New · NVIDIA · 8 GB</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>649</v>
+        <v>700</v>
       </c>
       <c r="E41" t="n">
         <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>649</v>
+        <v>700</v>
       </c>
       <c r="G41" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6-PCI-Express-4-0-Graphics-Card-PREORDER/124468386432?hash=item1cfae4da80:g:FN8AAOSwwSFfx7cA</t>
+          <t>https://www.ebay.com/itm/EVGA-GeForce-RTX-3060-Ti-FTW3-ULTRA-GAMING-Ready-to-ship/264961477720?hash=item3db0ef4c58:g:zhcAAOSwxVFfx8th</t>
         </is>
       </c>
     </row>
@@ -1761,7 +1761,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>New ListingNEW MSI Gaming GeForce RTX™ 3060 Ti GAMING X TRIO 8GB *IN HAND, FAST SHIP TODAY*</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6 PCI Express 4.0 Graphics Card *img*</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1770,20 +1770,20 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>699.99</v>
+        <v>500</v>
       </c>
       <c r="E42" t="n">
-        <v>0</v>
+        <v>3.8</v>
       </c>
       <c r="F42" t="n">
-        <v>699.99</v>
+        <v>503.8</v>
       </c>
       <c r="G42" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NEW-MSI-Gaming-GeForce-RTX-3060-Ti-GAMING-X-TRIO-8GB-IN-HAND-FAST-SHIP-TODAY/174542745756?hash=item28a38ef09c:g:PeoAAOSwxAFfx8Dn</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6-PCI-Express-4-0-Graphics-Card-img/393040327541?hash=item5b83077375:g:oIUAAOSwi3Bfx7gu</t>
         </is>
       </c>
     </row>
@@ -1793,12 +1793,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>New ListingZOTAC GAMING GeForce RTX 3060 Ti Twin Edge OC - ZT-A30610H-10M - Confirmed Order</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Brand New · ZOTAC · 8 GB</t>
+          <t>Brand New · Geforce · 8 GB</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1815,7 +1815,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/ZOTAC-GAMING-GeForce-RTX-3060-Ti-Twin-Edge-OC-ZT-A30610H-10M-Confirmed-Order/174542719758?hash=item28a38e8b0e:g:edkAAOSw9-9fx70Z</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card/264961483895?hash=item3db0ef6477:g:kdoAAOSw2PVfx7MO</t>
         </is>
       </c>
     </row>
@@ -1825,29 +1825,29 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>New ListingNvidia Geforce RTX 3060TI Founders Edition Picture. (read Desc)</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6 PCI Express 4.0 Graphics Card *PREORDER*</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Brand New</t>
+          <t>*PRE-ORDER! SHIPS OUT ON DECEMBER 8</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>399.99</v>
+        <v>649</v>
       </c>
       <c r="E44" t="n">
-        <v>4.9</v>
+        <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>404.89</v>
+        <v>649</v>
       </c>
       <c r="G44" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/Nvidia-Geforce-RTX-3060TI-Founders-Edition-Picture-read-Desc/203205997647?hash=item2f5005744f:g:KDcAAOSwqtJfx8SV</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6-PCI-Express-4-0-Graphics-Card-PREORDER/124468386432?hash=item1cfae4da80:g:FN8AAOSwwSFfx7cA</t>
         </is>
       </c>
     </row>
@@ -1857,7 +1857,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card *CONFIRMED*</t>
+          <t>New ListingNEW MSI Gaming GeForce RTX™ 3060 Ti GAMING X TRIO 8GB *IN HAND, FAST SHIP TODAY*</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1866,20 +1866,20 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>749.99</v>
+        <v>699.99</v>
       </c>
       <c r="E45" t="n">
         <v>0</v>
       </c>
       <c r="F45" t="n">
-        <v>749.99</v>
+        <v>699.99</v>
       </c>
       <c r="G45" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card-CONFIRMED/264961253005?hash=item3db0ebde8d:g:wiIAAOSwzPlfx6Dl</t>
+          <t>https://www.ebay.com/itm/NEW-MSI-Gaming-GeForce-RTX-3060-Ti-GAMING-X-TRIO-8GB-IN-HAND-FAST-SHIP-TODAY/174542745756?hash=item28a38ef09c:g:PeoAAOSwxAFfx8Dn</t>
         </is>
       </c>
     </row>
@@ -1889,29 +1889,29 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GEFORCE RTX 3060-TI Founders Edition -Printed image file</t>
+          <t>New ListingZOTAC GAMING GeForce RTX 3060 Ti Twin Edge OC - ZT-A30610H-10M - Confirmed Order</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Brand New · Geforce</t>
+          <t>Brand New · ZOTAC · 8 GB</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>350</v>
+        <v>650</v>
       </c>
       <c r="E46" t="n">
         <v>0</v>
       </c>
       <c r="F46" t="n">
-        <v>350</v>
+        <v>650</v>
       </c>
       <c r="G46" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GEFORCE-RTX-3060-TI-Founders-Edition-Printed-image-file/114554086719?hash=item1aabf4a53f:g:B2gAAOSw4h1fx8jO</t>
+          <t>https://www.ebay.com/itm/ZOTAC-GAMING-GeForce-RTX-3060-Ti-Twin-Edge-OC-ZT-A30610H-10M-Confirmed-Order/174542719758?hash=item28a38e8b0e:g:edkAAOSw9-9fx70Z</t>
         </is>
       </c>
     </row>
@@ -1921,29 +1921,29 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 TI Founders Edition PICTURE- DISCLAIMER READ DESCRIPTION</t>
+          <t>New ListingNvidia Geforce RTX 3060TI Founders Edition Picture. (read Desc)</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Brand New · NVIDIA · NVIDIA GeForce RTX 2080 Ti · 11GB</t>
+          <t>Brand New</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>389.99</v>
+        <v>399.99</v>
       </c>
       <c r="E47" t="n">
-        <v>0</v>
+        <v>4.9</v>
       </c>
       <c r="F47" t="n">
-        <v>389.99</v>
+        <v>404.89</v>
       </c>
       <c r="G47" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-TI-Founders-Edition-PICTURE-DISCLAIMER-READ-DESCRIPTION/353302705193?epid=9026714548&amp;hash=item52427b7429:g:EMEAAOSwildfx8V5</t>
+          <t>https://www.ebay.com/itm/Nvidia-Geforce-RTX-3060TI-Founders-Edition-Picture-read-Desc/203205997647?hash=item2f5005744f:g:KDcAAOSwqtJfx8SV</t>
         </is>
       </c>
     </row>
@@ -1953,29 +1953,29 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>New ListingNvidia GeForce RTX 3060 Ti Founders Edition - See Description</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card *CONFIRMED*</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Brand New · NVIDIA</t>
+          <t>Brand New · Geforce · 8 GB</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>399.99</v>
+        <v>749.99</v>
       </c>
       <c r="E48" t="n">
-        <v>19.99</v>
+        <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>419.98</v>
+        <v>749.99</v>
       </c>
       <c r="G48" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/Nvidia-GeForce-RTX-3060-Ti-Founders-Edition-See-Description/363204598737?hash=item5490ae5bd1:g:d1EAAOSwuDBfx8d9</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card-CONFIRMED/264961253005?hash=item3db0ebde8d:g:wiIAAOSwzPlfx6Dl</t>
         </is>
       </c>
     </row>
@@ -1985,29 +1985,29 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card  *Confirmed*</t>
+          <t>New ListingNVIDIA GEFORCE RTX 3060-TI Founders Edition -Printed image file</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Brand New · Geforce · 8 GB</t>
+          <t>Brand New · Geforce</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>725</v>
+        <v>350</v>
       </c>
       <c r="E49" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F49" t="n">
-        <v>750</v>
+        <v>350</v>
       </c>
       <c r="G49" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card-Confirmed/143869860779?hash=item217f4fdbab:g:XtMAAOSw4gRfx7U4</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GEFORCE-RTX-3060-TI-Founders-Edition-Printed-image-file/114554086719?hash=item1aabf4a53f:g:B2gAAOSw4h1fx8jO</t>
         </is>
       </c>
     </row>
@@ -2017,29 +2017,29 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t xml:space="preserve">New ListingNVIDIA FOUNDERS EDITION GeForce RTX 3060 Ti  Graphics Card </t>
+          <t>New ListingNVIDIA GeForce RTX 3060 TI Founders Edition PICTURE- DISCLAIMER READ DESCRIPTION</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Brand New · Geforce · 8 GB</t>
+          <t>Brand New · NVIDIA · NVIDIA GeForce RTX 2080 Ti · 11GB</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>699.99</v>
+        <v>389.99</v>
       </c>
       <c r="E50" t="n">
-        <v>14.75</v>
+        <v>0</v>
       </c>
       <c r="F50" t="n">
-        <v>714.74</v>
+        <v>389.99</v>
       </c>
       <c r="G50" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-FOUNDERS-EDITION-GeForce-RTX-3060-Ti-Graphics-Card/393040386273?hash=item5b830858e1:g:Ps0AAOSw8DNfx8NH</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-TI-Founders-Edition-PICTURE-DISCLAIMER-READ-DESCRIPTION/353302705193?epid=9026714548&amp;hash=item52427b7429:g:EMEAAOSwildfx8V5</t>
         </is>
       </c>
     </row>
@@ -2049,29 +2049,29 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB 4.0 Founder's Edition Graphics Card</t>
+          <t>New ListingNvidia GeForce RTX 3060 Ti Founders Edition - See Description</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Brand New · NVIDIA · 8 GB</t>
+          <t>Brand New · NVIDIA</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>725</v>
+        <v>399.99</v>
       </c>
       <c r="E51" t="n">
-        <v>0</v>
+        <v>19.99</v>
       </c>
       <c r="F51" t="n">
-        <v>725</v>
+        <v>419.98</v>
       </c>
       <c r="G51" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-4-0-Founders-Edition-Graphics-Card/224261547052?hash=item343707a42c:g:27UAAOSwVFhfx8X~</t>
+          <t>https://www.ebay.com/itm/Nvidia-GeForce-RTX-3060-Ti-Founders-Edition-See-Description/363204598737?hash=item5490ae5bd1:g:d1EAAOSwuDBfx8d9</t>
         </is>
       </c>
     </row>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card  *Confirmed*</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2090,20 +2090,20 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>650</v>
+        <v>725</v>
       </c>
       <c r="E52" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F52" t="n">
-        <v>650</v>
+        <v>750</v>
       </c>
       <c r="G52" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card/254796370765?hash=item3b530c134d:g:kdoAAOSw2PVfx7MO</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card-Confirmed/143869860779?hash=item217f4fdbab:g:XtMAAOSw4gRfx7U4</t>
         </is>
       </c>
     </row>
@@ -2113,29 +2113,29 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6 PCI Express 4.0 Graphics Card</t>
+          <t xml:space="preserve">New ListingNVIDIA FOUNDERS EDITION GeForce RTX 3060 Ti  Graphics Card </t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Brand New · Nvida · 8 GB</t>
+          <t>Brand New · Geforce · 8 GB</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>680</v>
+        <v>699.99</v>
       </c>
       <c r="E53" t="n">
-        <v>12.55</v>
+        <v>14.75</v>
       </c>
       <c r="F53" t="n">
-        <v>692.55</v>
+        <v>714.74</v>
       </c>
       <c r="G53" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6-PCI-Express-4-0-Graphics-Card/233805723853?hash=item366fe838cd:g:Ul0AAOSw7b9fx8WT</t>
+          <t>https://www.ebay.com/itm/NVIDIA-FOUNDERS-EDITION-GeForce-RTX-3060-Ti-Graphics-Card/393040386273?hash=item5b830858e1:g:Ps0AAOSw8DNfx8NH</t>
         </is>
       </c>
     </row>
@@ -2145,29 +2145,29 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB Founders Edition *CONFIRMED*</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB 4.0 Founder's Edition Graphics Card</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Brand New · Geforce · 8 GB</t>
+          <t>Brand New · NVIDIA · 8 GB</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>675</v>
+        <v>725</v>
       </c>
       <c r="E54" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F54" t="n">
-        <v>690</v>
+        <v>725</v>
       </c>
       <c r="G54" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-Founders-Edition-CONFIRMED/303792863240?hash=item46bb773808:g:ol8AAOSwl5hfx7yO</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-4-0-Founders-Edition-Graphics-Card/224261547052?hash=item343707a42c:g:27UAAOSwVFhfx8X~</t>
         </is>
       </c>
     </row>
@@ -2177,29 +2177,29 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>New ListingEvga Rtx 3060ti Ftw3 Ultra CAN SHIP TODAY!</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Open Box · EVGA</t>
+          <t>Brand New · Geforce · 8 GB</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>675</v>
+        <v>650</v>
       </c>
       <c r="E55" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F55" t="n">
-        <v>685</v>
+        <v>650</v>
       </c>
       <c r="G55" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/Evga-Rtx-3060ti-Ftw3-Ultra-CAN-SHIP-TODAY/224261505370?hash=item343707015a:g:m90AAOSwaDRfx7xM</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card/254796370765?hash=item3b530c134d:g:kdoAAOSw2PVfx7MO</t>
         </is>
       </c>
     </row>
@@ -2209,7 +2209,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6 PCI Express 4.0 Graphics Card order confirm</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6 PCI Express 4.0 Graphics Card</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2218,20 +2218,20 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>649.99</v>
+        <v>680</v>
       </c>
       <c r="E56" t="n">
-        <v>0</v>
+        <v>12.55</v>
       </c>
       <c r="F56" t="n">
-        <v>649.99</v>
+        <v>692.55</v>
       </c>
       <c r="G56" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6-PCI-Express-4-0-Graphics-Card-order-confirm/164553109041?hash=item2650212e31:g:1wAAAOSwdmJfx8Oq</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6-PCI-Express-4-0-Graphics-Card/233805723853?hash=item366fe838cd:g:Ul0AAOSw7b9fx8WT</t>
         </is>
       </c>
     </row>
@@ -2241,7 +2241,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>New ListingSEALED ASUS TUF Nvidia Geforce RTX 3060 ti OC Edition Graphics Card 8GB IN HAND</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB Founders Edition *CONFIRMED*</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2250,20 +2250,20 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>849.99</v>
+        <v>675</v>
       </c>
       <c r="E57" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F57" t="n">
-        <v>849.99</v>
+        <v>690</v>
       </c>
       <c r="G57" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/SEALED-ASUS-TUF-Nvidia-Geforce-RTX-3060-ti-OC-Edition-Graphics-Card-8GB-IN-HAND/264961352257?hash=item3db0ed6241:g:SqQAAOSwnFJfx7Sw</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-Founders-Edition-CONFIRMED/303792863240?hash=item46bb773808:g:ol8AAOSwl5hfx7yO</t>
         </is>
       </c>
     </row>
@@ -2273,29 +2273,29 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t xml:space="preserve">New ListingNEW NVIDIA GEFORCE RTX 3060-TI FOUNDERS EDITION- image file Brand New · </t>
+          <t>New ListingEvga Rtx 3060ti Ftw3 Ultra CAN SHIP TODAY!</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Brand New · Geforce · 8 GB</t>
+          <t>Open Box · EVGA</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>400</v>
+        <v>675</v>
       </c>
       <c r="E58" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F58" t="n">
-        <v>400</v>
+        <v>685</v>
       </c>
       <c r="G58" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NEW-NVIDIA-GEFORCE-RTX-3060-TI-FOUNDERS-EDITION-image-file-Brand-New/203205986943?hash=item2f50054a7f:g:FGYAAOSwLq1fx8Kn</t>
+          <t>https://www.ebay.com/itm/Evga-Rtx-3060ti-Ftw3-Ultra-CAN-SHIP-TODAY/224261505370?hash=item343707015a:g:m90AAOSwaDRfx7xM</t>
         </is>
       </c>
     </row>
@@ -2305,29 +2305,29 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti Founders Edition as picture</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6 PCI Express 4.0 Graphics Card order confirm</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Brand New · Geforce · 8 GB</t>
+          <t>Brand New · Nvida · 8 GB</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>730</v>
+        <v>649.99</v>
       </c>
       <c r="E59" t="n">
         <v>0</v>
       </c>
       <c r="F59" t="n">
-        <v>730</v>
+        <v>649.99</v>
       </c>
       <c r="G59" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-Founders-Edition-as-picture/143869396844?hash=item217f48c76c:g:ZgAAAOSwlRVfxymZ</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6-PCI-Express-4-0-Graphics-Card-order-confirm/164553109041?hash=item2650212e31:g:1wAAAOSwdmJfx8Oq</t>
         </is>
       </c>
     </row>
@@ -2337,7 +2337,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card *SHIPS 12/9*</t>
+          <t>New ListingSEALED ASUS TUF Nvidia Geforce RTX 3060 ti OC Edition Graphics Card 8GB IN HAND</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2346,20 +2346,20 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>699.99</v>
+        <v>849.99</v>
       </c>
       <c r="E60" t="n">
         <v>0</v>
       </c>
       <c r="F60" t="n">
-        <v>699.99</v>
+        <v>849.99</v>
       </c>
       <c r="G60" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card-SHIPS-12-9/154223672561?hash=item23e8727cf1:g:0oUAAOSwwCNfx72L</t>
+          <t>https://www.ebay.com/itm/SEALED-ASUS-TUF-Nvidia-Geforce-RTX-3060-ti-OC-Edition-Graphics-Card-8GB-IN-HAND/264961352257?hash=item3db0ed6241:g:SqQAAOSwnFJfx7Sw</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>New ListingNvidia Geforce RTX 3060 TI Founders Edition Graphics Card *Will ship by Dec 9*</t>
+          <t xml:space="preserve">New ListingNEW NVIDIA GEFORCE RTX 3060-TI FOUNDERS EDITION- image file Brand New · </t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2378,20 +2378,20 @@
         </is>
       </c>
       <c r="D61" t="n">
-        <v>635</v>
+        <v>400</v>
       </c>
       <c r="E61" t="n">
-        <v>10.55</v>
+        <v>0</v>
       </c>
       <c r="F61" t="n">
-        <v>645.55</v>
+        <v>400</v>
       </c>
       <c r="G61" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/Nvidia-Geforce-RTX-3060-TI-Founders-Edition-Graphics-Card-Will-ship-by-Dec-9/284101484442?hash=item4225c49f9a:g:TGwAAOSwktpfx8Cz</t>
+          <t>https://www.ebay.com/itm/NEW-NVIDIA-GEFORCE-RTX-3060-TI-FOUNDERS-EDITION-image-file-Brand-New/203205986943?hash=item2f50054a7f:g:FGYAAOSwLq1fx8Kn</t>
         </is>
       </c>
     </row>
@@ -2401,29 +2401,29 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GEFORCE RTX 3060 Ti ASUS TUF BRAND NEW IN HAND SHIP FAST</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti Founders Edition as picture</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Brand New · ASUS</t>
+          <t>Brand New · Geforce · 8 GB</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>709.99</v>
+        <v>730</v>
       </c>
       <c r="E62" t="n">
         <v>0</v>
       </c>
       <c r="F62" t="n">
-        <v>709.99</v>
+        <v>730</v>
       </c>
       <c r="G62" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GEFORCE-RTX-3060-Ti-ASUS-TUF-BRAND-NEW-IN-HAND-SHIP-FAST/284101479071?hash=item4225c48a9f:g:U~4AAOSwg-xfx76E</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-Founders-Edition-as-picture/143869396844?hash=item217f48c76c:g:ZgAAAOSwlRVfxymZ</t>
         </is>
       </c>
     </row>
@@ -2433,29 +2433,29 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB Founder's Edition</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card *SHIPS 12/9*</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Brand New · NVIDIA · 8 GB</t>
+          <t>Brand New · Geforce · 8 GB</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>649.99</v>
+        <v>699.99</v>
       </c>
       <c r="E63" t="n">
         <v>0</v>
       </c>
       <c r="F63" t="n">
-        <v>649.99</v>
+        <v>699.99</v>
       </c>
       <c r="G63" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-Founders-Edition/264961438388?hash=item3db0eeb2b4:g:cUIAAOSwbVVfx7sA</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card-SHIPS-12-9/154223672561?hash=item23e8727cf1:g:0oUAAOSwwCNfx72L</t>
         </is>
       </c>
     </row>
@@ -2465,29 +2465,29 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GEFORCE RTX 3060-TI Founders Edition -Printed image file</t>
+          <t>New ListingNvidia Geforce RTX 3060 TI Founders Edition Graphics Card *Will ship by Dec 9*</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Brand New · Geforce</t>
+          <t>Brand New · Geforce · 8 GB</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>350</v>
+        <v>635</v>
       </c>
       <c r="E64" t="n">
-        <v>0</v>
+        <v>10.55</v>
       </c>
       <c r="F64" t="n">
-        <v>350</v>
+        <v>645.55</v>
       </c>
       <c r="G64" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GEFORCE-RTX-3060-TI-Founders-Edition-Printed-image-file/203205981351?hash=item2f500534a7:g:ziMAAOSwdQhfx8GZ</t>
+          <t>https://www.ebay.com/itm/Nvidia-Geforce-RTX-3060-TI-Founders-Edition-Graphics-Card-Will-ship-by-Dec-9/284101484442?hash=item4225c49f9a:g:TGwAAOSwktpfx8Cz</t>
         </is>
       </c>
     </row>
@@ -2497,29 +2497,29 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>New ListingGIGABYTE AORUS GeForce RTX 3060 Ti (Confirmed Order)</t>
+          <t>New ListingNVIDIA GEFORCE RTX 3060 Ti ASUS TUF BRAND NEW IN HAND SHIP FAST</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Brand New · GIGABYTE · 8 GB</t>
+          <t>Brand New · ASUS</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>699</v>
+        <v>709.99</v>
       </c>
       <c r="E65" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F65" t="n">
-        <v>713</v>
+        <v>709.99</v>
       </c>
       <c r="G65" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/GIGABYTE-AORUS-GeForce-RTX-3060-Ti-Confirmed-Order/264961262245?hash=item3db0ec02a5:g:PwkAAOSwT5Zfx6EJ</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GEFORCE-RTX-3060-Ti-ASUS-TUF-BRAND-NEW-IN-HAND-SHIP-FAST/284101479071?hash=item4225c48a9f:g:U~4AAOSwg-xfx76E</t>
         </is>
       </c>
     </row>
@@ -2529,29 +2529,29 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6 Graphics Card PRE ORDER CONFIRMED BEST BUY</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB Founder's Edition</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Brand New · Geforce · 8 GB</t>
+          <t>Brand New · NVIDIA · 8 GB</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>600</v>
+        <v>649.99</v>
       </c>
       <c r="E66" t="n">
-        <v>23.85</v>
+        <v>0</v>
       </c>
       <c r="F66" t="n">
-        <v>623.85</v>
+        <v>649.99</v>
       </c>
       <c r="G66" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6-Graphics-Card-PRE-ORDER-CONFIRMED-BEST-BUY/402587089981?hash=item5dbc0f7c3d:g:8L8AAOSwNm1fx7ou</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-Founders-Edition/264961438388?hash=item3db0eeb2b4:g:cUIAAOSwbVVfx7sA</t>
         </is>
       </c>
     </row>
@@ -2561,29 +2561,29 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6 PCI Express 4.0 Graphics Card order confirm</t>
+          <t>New ListingNVIDIA GEFORCE RTX 3060-TI Founders Edition -Printed image file</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Brand New · Nvida · 8 GB</t>
+          <t>Brand New · Geforce</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>699</v>
+        <v>350</v>
       </c>
       <c r="E67" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F67" t="n">
-        <v>708</v>
+        <v>350</v>
       </c>
       <c r="G67" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6-PCI-Express-4-0-Graphics-Card-order-confirm/114553979538?hash=item1aabf30292:g:SnkAAOSwSBpfx7Zr</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GEFORCE-RTX-3060-TI-Founders-Edition-Printed-image-file/203205981351?hash=item2f500534a7:g:ziMAAOSwdQhfx8GZ</t>
         </is>
       </c>
     </row>
@@ -2593,29 +2593,29 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card  *PRE ORDER*</t>
+          <t>New ListingGIGABYTE AORUS GeForce RTX 3060 Ti (Confirmed Order)</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Brand New · Geforce · 8 GB</t>
+          <t>Brand New · GIGABYTE · 8 GB</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>650</v>
+        <v>699</v>
       </c>
       <c r="E68" t="n">
-        <v>10.95</v>
+        <v>14</v>
       </c>
       <c r="F68" t="n">
-        <v>660.95</v>
+        <v>713</v>
       </c>
       <c r="G68" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card-PRE-ORDER/393039373551?hash=item5b82f8e4ef:g:r-EAAOSw~xBfxudP</t>
+          <t>https://www.ebay.com/itm/GIGABYTE-AORUS-GeForce-RTX-3060-Ti-Confirmed-Order/264961262245?hash=item3db0ec02a5:g:PwkAAOSwT5Zfx6EJ</t>
         </is>
       </c>
     </row>
@@ -2625,29 +2625,29 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB Founder's Edition</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6 Graphics Card PRE ORDER CONFIRMED BEST BUY</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Brand New · NVIDIA · 8 GB</t>
+          <t>Brand New · Geforce · 8 GB</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>649.99</v>
+        <v>600</v>
       </c>
       <c r="E69" t="n">
-        <v>0</v>
+        <v>23.85</v>
       </c>
       <c r="F69" t="n">
-        <v>649.99</v>
+        <v>623.85</v>
       </c>
       <c r="G69" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-Founders-Edition/264961409275?hash=item3db0ee40fb:g:cUIAAOSwbVVfx7sA</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6-Graphics-Card-PRE-ORDER-CONFIRMED-BEST-BUY/402587089981?hash=item5dbc0f7c3d:g:8L8AAOSwNm1fx7ou</t>
         </is>
       </c>
     </row>
@@ -2657,29 +2657,29 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card  SHIPS 12/9</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6 PCI Express 4.0 Graphics Card order confirm</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Brand New · Geforce · 8 GB</t>
+          <t>Brand New · Nvida · 8 GB</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>649.99</v>
+        <v>699</v>
       </c>
       <c r="E70" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F70" t="n">
-        <v>649.99</v>
+        <v>708</v>
       </c>
       <c r="G70" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card-SHIPS-12-9/254796382625?hash=item3b530c41a1:g:GC0AAOSwEJdfx7V7</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6-PCI-Express-4-0-Graphics-Card-order-confirm/114553979538?hash=item1aabf30292:g:SnkAAOSwSBpfx7Zr</t>
         </is>
       </c>
     </row>
@@ -2689,7 +2689,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>New ListingGeForce RTX 3060 TI 8GB GDDR6 Founders Edition PCI Express 4.0  Printed Image</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card  *PRE ORDER*</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2698,20 +2698,20 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>399</v>
+        <v>650</v>
       </c>
       <c r="E71" t="n">
-        <v>0</v>
+        <v>10.95</v>
       </c>
       <c r="F71" t="n">
-        <v>399</v>
+        <v>660.95</v>
       </c>
       <c r="G71" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/GeForce-RTX-3060-TI-8GB-GDDR6-Founders-Edition-PCI-Express-4-0-Printed-Image/383839080458?hash=item595e97900a:g:-GQAAOSwTcdfx7u-</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card-PRE-ORDER/393039373551?hash=item5b82f8e4ef:g:r-EAAOSw~xBfxudP</t>
         </is>
       </c>
     </row>
@@ -2721,29 +2721,29 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t xml:space="preserve">New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card  *PRE ORDER* </t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB Founder's Edition</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Brand New · Geforce · 8 GB</t>
+          <t>Brand New · NVIDIA · 8 GB</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>675</v>
+        <v>649.99</v>
       </c>
       <c r="E72" t="n">
         <v>0</v>
       </c>
       <c r="F72" t="n">
-        <v>675</v>
+        <v>649.99</v>
       </c>
       <c r="G72" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card-PRE-ORDER/174542692794?hash=item28a38e21ba:g:sMkAAOSwY1Ffx7T-</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-Founders-Edition/264961409275?hash=item3db0ee40fb:g:cUIAAOSwbVVfx7sA</t>
         </is>
       </c>
     </row>
@@ -2753,7 +2753,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6 PCI Express 4.0 Graphics</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card  SHIPS 12/9</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2762,20 +2762,20 @@
         </is>
       </c>
       <c r="D73" t="n">
-        <v>638.95</v>
+        <v>649.99</v>
       </c>
       <c r="E73" t="n">
         <v>0</v>
       </c>
       <c r="F73" t="n">
-        <v>638.95</v>
+        <v>649.99</v>
       </c>
       <c r="G73" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6-PCI-Express-4-0-Graphics/114554009569?hash=item1aabf377e1:g:-4EAAOSwk4Jfx7vd</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card-SHIPS-12-9/254796382625?hash=item3b530c41a1:g:GC0AAOSwEJdfx7V7</t>
         </is>
       </c>
     </row>
@@ -2785,7 +2785,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card PRE ORDER</t>
+          <t>New ListingGeForce RTX 3060 TI 8GB GDDR6 Founders Edition PCI Express 4.0  Printed Image</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2794,20 +2794,20 @@
         </is>
       </c>
       <c r="D74" t="n">
-        <v>600</v>
+        <v>399</v>
       </c>
       <c r="E74" t="n">
         <v>0</v>
       </c>
       <c r="F74" t="n">
-        <v>600</v>
+        <v>399</v>
       </c>
       <c r="G74" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card-PRE-ORDER/193776623719?hash=item2d1dfca067:g:OWkAAOSwUepfx7tx</t>
+          <t>https://www.ebay.com/itm/GeForce-RTX-3060-TI-8GB-GDDR6-Founders-Edition-PCI-Express-4-0-Printed-Image/383839080458?hash=item595e97900a:g:-GQAAOSwTcdfx7u-</t>
         </is>
       </c>
     </row>
@@ -2817,7 +2817,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card</t>
+          <t xml:space="preserve">New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card  *PRE ORDER* </t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2826,20 +2826,20 @@
         </is>
       </c>
       <c r="D75" t="n">
-        <v>625</v>
+        <v>675</v>
       </c>
       <c r="E75" t="n">
-        <v>12.26</v>
+        <v>0</v>
       </c>
       <c r="F75" t="n">
-        <v>637.26</v>
+        <v>675</v>
       </c>
       <c r="G75" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card/224261501324?hash=item343706f18c:g:AN4AAOSw3o5fx7vi</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card-PRE-ORDER/174542692794?hash=item28a38e21ba:g:sMkAAOSwY1Ffx7T-</t>
         </is>
       </c>
     </row>
@@ -2849,7 +2849,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>New ListingNvidia Geforce RTX 3060 TI Founders Edition Graphics Card - *SHIP OUT TODAY*</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6 PCI Express 4.0 Graphics</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2858,20 +2858,20 @@
         </is>
       </c>
       <c r="D76" t="n">
-        <v>740</v>
+        <v>638.95</v>
       </c>
       <c r="E76" t="n">
-        <v>14.4</v>
+        <v>0</v>
       </c>
       <c r="F76" t="n">
-        <v>754.4</v>
+        <v>638.95</v>
       </c>
       <c r="G76" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/Nvidia-Geforce-RTX-3060-TI-Founders-Edition-Graphics-Card-SHIP-OUT-TODAY/353302522987?hash=item524278ac6b:g:65kAAOSwuRxfx740</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6-PCI-Express-4-0-Graphics/114554009569?hash=item1aabf377e1:g:-4EAAOSwk4Jfx7vd</t>
         </is>
       </c>
     </row>
@@ -2881,29 +2881,29 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB picture (Read description)</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card PRE ORDER</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Brand New · NVIDIA · 8 GB</t>
+          <t>Brand New · Geforce · 8 GB</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>399.99</v>
+        <v>600</v>
       </c>
       <c r="E77" t="n">
-        <v>6.75</v>
+        <v>0</v>
       </c>
       <c r="F77" t="n">
-        <v>406.74</v>
+        <v>600</v>
       </c>
       <c r="G77" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-picture-Read-description/303792828837?hash=item46bb76b1a5:g:lxAAAOSw69Ffx7MB</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card-PRE-ORDER/193776623719?hash=item2d1dfca067:g:OWkAAOSwUepfx7tx</t>
         </is>
       </c>
     </row>
@@ -2913,29 +2913,29 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>New ListingNEW NVIDIA GEFORCE RTX 3060-TI FOUNDERS EDITION- Printed image file</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Brand New · Geforce</t>
+          <t>Brand New · Geforce · 8 GB</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>400</v>
+        <v>625</v>
       </c>
       <c r="E78" t="n">
-        <v>0</v>
+        <v>12.26</v>
       </c>
       <c r="F78" t="n">
-        <v>400</v>
+        <v>637.26</v>
       </c>
       <c r="G78" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NEW-NVIDIA-GEFORCE-RTX-3060-TI-FOUNDERS-EDITION-Printed-image-file/303792759105?hash=item46bb75a141:g:CCAAAOSwZDdfx7rc</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card/224261501324?hash=item343706f18c:g:AN4AAOSw3o5fx7vi</t>
         </is>
       </c>
     </row>
@@ -2945,7 +2945,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>New ListingNvidia Geforce RTX 3060 ti Graphics Card 8GB GDDR6</t>
+          <t>New ListingNvidia Geforce RTX 3060 TI Founders Edition Graphics Card - *SHIP OUT TODAY*</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2954,20 +2954,20 @@
         </is>
       </c>
       <c r="D79" t="n">
-        <v>450</v>
+        <v>740</v>
       </c>
       <c r="E79" t="n">
-        <v>0</v>
+        <v>14.4</v>
       </c>
       <c r="F79" t="n">
-        <v>450</v>
+        <v>754.4</v>
       </c>
       <c r="G79" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/Nvidia-Geforce-RTX-3060-ti-Graphics-Card-8GB-GDDR6/233805464152?hash=item366fe44258:g:JmkAAOSw5ydfx6a-</t>
+          <t>https://www.ebay.com/itm/Nvidia-Geforce-RTX-3060-TI-Founders-Edition-Graphics-Card-SHIP-OUT-TODAY/353302522987?hash=item524278ac6b:g:65kAAOSwuRxfx740</t>
         </is>
       </c>
     </row>
@@ -2977,29 +2977,29 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB picture (Read description)</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Brand New · Geforce · 8 GB</t>
+          <t>Brand New · NVIDIA · 8 GB</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>649.98</v>
+        <v>399.99</v>
       </c>
       <c r="E80" t="n">
-        <v>0</v>
+        <v>6.75</v>
       </c>
       <c r="F80" t="n">
-        <v>649.98</v>
+        <v>406.74</v>
       </c>
       <c r="G80" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card/233805640616?hash=item366fe6f3a8:g:CC8AAOSwHpZfx7Ue</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-picture-Read-description/303792828837?hash=item46bb76b1a5:g:lxAAAOSw69Ffx7MB</t>
         </is>
       </c>
     </row>
@@ -3009,29 +3009,29 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card  *SHIPS 12/9*</t>
+          <t>New ListingNEW NVIDIA GEFORCE RTX 3060-TI FOUNDERS EDITION- Printed image file</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Brand New · Geforce · 8 GB</t>
+          <t>Brand New · Geforce</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>699.99</v>
+        <v>400</v>
       </c>
       <c r="E81" t="n">
         <v>0</v>
       </c>
       <c r="F81" t="n">
-        <v>699.99</v>
+        <v>400</v>
       </c>
       <c r="G81" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card-SHIPS-12-9/203205928048?hash=item2f50046470:g:1ykAAOSwAu5fx7Q1</t>
+          <t>https://www.ebay.com/itm/NEW-NVIDIA-GEFORCE-RTX-3060-TI-FOUNDERS-EDITION-Printed-image-file/303792759105?hash=item46bb75a141:g:CCAAAOSwZDdfx7rc</t>
         </is>
       </c>
     </row>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card  *IN HAND*</t>
+          <t>New ListingNvidia Geforce RTX 3060 ti Graphics Card 8GB GDDR6</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3050,20 +3050,20 @@
         </is>
       </c>
       <c r="D82" t="n">
-        <v>560</v>
+        <v>450</v>
       </c>
       <c r="E82" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F82" t="n">
-        <v>575</v>
+        <v>450</v>
       </c>
       <c r="G82" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card-IN-HAND/353302604714?hash=item524279ebaa:g:oF4AAOSw31Jfx7gM</t>
+          <t>https://www.ebay.com/itm/Nvidia-Geforce-RTX-3060-ti-Graphics-Card-8GB-GDDR6/233805464152?hash=item366fe44258:g:JmkAAOSw5ydfx6a-</t>
         </is>
       </c>
     </row>
@@ -3073,29 +3073,29 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB Founders Edition *CONFIRMED*</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Brand New · NVIDIA · 8 GB</t>
+          <t>Brand New · Geforce · 8 GB</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>650</v>
+        <v>649.98</v>
       </c>
       <c r="E83" t="n">
         <v>0</v>
       </c>
       <c r="F83" t="n">
-        <v>650</v>
+        <v>649.98</v>
       </c>
       <c r="G83" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-Founders-Edition-CONFIRMED/383839017491?hash=item595e969a13:g:QTMAAOSwa6Jfx7Mx</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card/233805640616?hash=item366fe6f3a8:g:CC8AAOSwHpZfx7Ue</t>
         </is>
       </c>
     </row>
@@ -3105,7 +3105,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t xml:space="preserve">New ListingNVIDIA FOUNDERS EDITION GeForce RTX 3060 Ti  Graphics Card </t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card  *SHIPS 12/9*</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3114,20 +3114,20 @@
         </is>
       </c>
       <c r="D84" t="n">
-        <v>669.99</v>
+        <v>699.99</v>
       </c>
       <c r="E84" t="n">
         <v>0</v>
       </c>
       <c r="F84" t="n">
-        <v>669.99</v>
+        <v>699.99</v>
       </c>
       <c r="G84" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-FOUNDERS-EDITION-GeForce-RTX-3060-Ti-Graphics-Card/383839029320?hash=item595e96c848:g:UWEAAOSwpfxfx7UJ</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card-SHIPS-12-9/203205928048?hash=item2f50046470:g:1ykAAOSwAu5fx7Q1</t>
         </is>
       </c>
     </row>
@@ -3137,29 +3137,29 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>New ListingEVGA GEFORCE RTX 3060 TI XC 8GB GDDR6 METAL BACKPLATE (***IN HAND***)</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card  *IN HAND*</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Brand New · EVGA · 8 GB</t>
+          <t>Brand New · Geforce · 8 GB</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>650</v>
+        <v>560</v>
       </c>
       <c r="E85" t="n">
-        <v>9.9</v>
+        <v>15</v>
       </c>
       <c r="F85" t="n">
-        <v>659.9</v>
+        <v>575</v>
       </c>
       <c r="G85" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/EVGA-GEFORCE-RTX-3060-TI-XC-8GB-GDDR6-METAL-BACKPLATE-IN-HAND/363204516827?hash=item5490ad1bdb:g:LN4AAOSwPGBfx7Nc</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card-IN-HAND/353302604714?hash=item524279ebaa:g:oF4AAOSw31Jfx7gM</t>
         </is>
       </c>
     </row>
@@ -3169,29 +3169,29 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphic Card Order Confirmed</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB Founders Edition *CONFIRMED*</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Brand New · Geforce · 8 GB</t>
+          <t>Brand New · NVIDIA · 8 GB</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>629</v>
+        <v>650</v>
       </c>
       <c r="E86" t="n">
         <v>0</v>
       </c>
       <c r="F86" t="n">
-        <v>629</v>
+        <v>650</v>
       </c>
       <c r="G86" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphic-Card-Order-Confirmed/233805612562?hash=item366fe68612:g:pJIAAOSwwfdfx7Ma</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-Founders-Edition-CONFIRMED/383839017491?hash=item595e969a13:g:QTMAAOSwa6Jfx7Mx</t>
         </is>
       </c>
     </row>
@@ -3201,7 +3201,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6 PCI Express 4.0 Graphics Card *PREORDER*</t>
+          <t xml:space="preserve">New ListingNVIDIA FOUNDERS EDITION GeForce RTX 3060 Ti  Graphics Card </t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3210,20 +3210,20 @@
         </is>
       </c>
       <c r="D87" t="n">
-        <v>649.99</v>
+        <v>669.99</v>
       </c>
       <c r="E87" t="n">
         <v>0</v>
       </c>
       <c r="F87" t="n">
-        <v>649.99</v>
+        <v>669.99</v>
       </c>
       <c r="G87" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6-PCI-Express-4-0-Graphics-Card-PREORDER/133594868564?hash=item1f1adfeb54:g:DIYAAOSwzq5fx7Tl</t>
+          <t>https://www.ebay.com/itm/NVIDIA-FOUNDERS-EDITION-GeForce-RTX-3060-Ti-Graphics-Card/383839029320?hash=item595e96c848:g:UWEAAOSwpfxfx7UJ</t>
         </is>
       </c>
     </row>
@@ -3233,29 +3233,29 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t xml:space="preserve">New ListingNEW NVIDIA GEFORCE RTX 3060-TI FOUNDERS EDITION- Printed image file Brand New · </t>
+          <t>New ListingEVGA GEFORCE RTX 3060 TI XC 8GB GDDR6 METAL BACKPLATE (***IN HAND***)</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Brand New · Geforce</t>
+          <t>Brand New · EVGA · 8 GB</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>400</v>
+        <v>650</v>
       </c>
       <c r="E88" t="n">
-        <v>0</v>
+        <v>9.9</v>
       </c>
       <c r="F88" t="n">
-        <v>400</v>
+        <v>659.9</v>
       </c>
       <c r="G88" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NEW-NVIDIA-GEFORCE-RTX-3060-TI-FOUNDERS-EDITION-Printed-image-file-Brand-New/114553970353?hash=item1aabf2deb1:g:vRAAAOSw6qdfx7VX</t>
+          <t>https://www.ebay.com/itm/EVGA-GEFORCE-RTX-3060-TI-XC-8GB-GDDR6-METAL-BACKPLATE-IN-HAND/363204516827?hash=item5490ad1bdb:g:LN4AAOSwPGBfx7Nc</t>
         </is>
       </c>
     </row>
@@ -3265,29 +3265,29 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA Geforce RTX 3060 Ti 8GB (Read description)</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphic Card Order Confirmed</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Brand New · NVIDIA</t>
+          <t>Brand New · Geforce · 8 GB</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>430</v>
+        <v>629</v>
       </c>
       <c r="E89" t="n">
         <v>0</v>
       </c>
       <c r="F89" t="n">
-        <v>430</v>
+        <v>629</v>
       </c>
       <c r="G89" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-Geforce-RTX-3060-Ti-8GB-Read-description/233805519514?hash=item366fe51a9a:g:AmwAAOSwh-dfx6m4</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphic-Card-Order-Confirmed/233805612562?hash=item366fe68612:g:pJIAAOSwwfdfx7Ma</t>
         </is>
       </c>
     </row>
@@ -3297,7 +3297,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>New ListingNEW NVIDIA GEFORCE RTX 3060-TI FOUNDERS EDITION- Printed image file</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6 PCI Express 4.0 Graphics Card *PREORDER*</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3306,20 +3306,20 @@
         </is>
       </c>
       <c r="D90" t="n">
-        <v>450</v>
+        <v>649.99</v>
       </c>
       <c r="E90" t="n">
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="F90" t="n">
-        <v>457.5</v>
+        <v>649.99</v>
       </c>
       <c r="G90" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NEW-NVIDIA-GEFORCE-RTX-3060-TI-FOUNDERS-EDITION-Printed-image-file/224261447352?hash=item3437061eb8:g:KGgAAOSwlOJfx6vb</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6-PCI-Express-4-0-Graphics-Card-PREORDER/133594868564?hash=item1f1adfeb54:g:DIYAAOSwzq5fx7Tl</t>
         </is>
       </c>
     </row>
@@ -3329,29 +3329,29 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>New ListingNvidia Geforce RTX 3060 ti Founders Edition Graphics Card 8GB GDDR6 READ</t>
+          <t xml:space="preserve">New ListingNEW NVIDIA GEFORCE RTX 3060-TI FOUNDERS EDITION- Printed image file Brand New · </t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Brand New · Geforce · 8 GB</t>
+          <t>Brand New · Geforce</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="E91" t="n">
         <v>0</v>
       </c>
       <c r="F91" t="n">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="G91" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/Nvidia-Geforce-RTX-3060-ti-Founders-Edition-Graphics-Card-8GB-GDDR6-READ/383839013705?hash=item595e968b49:g:~v0AAOSw3Vpfx7Fu</t>
+          <t>https://www.ebay.com/itm/NEW-NVIDIA-GEFORCE-RTX-3060-TI-FOUNDERS-EDITION-Printed-image-file-Brand-New/114553970353?hash=item1aabf2deb1:g:vRAAAOSw6qdfx7VX</t>
         </is>
       </c>
     </row>
@@ -3361,29 +3361,29 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>New ListingGeforce RTX 3060 ti Founder Edition</t>
+          <t>New ListingNVIDIA Geforce RTX 3060 Ti 8GB (Read description)</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Brand New · Geforce · 8 GB</t>
+          <t>Brand New · NVIDIA</t>
         </is>
       </c>
       <c r="D92" t="n">
-        <v>795</v>
+        <v>430</v>
       </c>
       <c r="E92" t="n">
-        <v>10.9</v>
+        <v>0</v>
       </c>
       <c r="F92" t="n">
-        <v>805.9</v>
+        <v>430</v>
       </c>
       <c r="G92" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/Geforce-RTX-3060-ti-Founder-Edition/303792758346?hash=item46bb759e4a:g:~FcAAOSw5Clfx6uE</t>
+          <t>https://www.ebay.com/itm/NVIDIA-Geforce-RTX-3060-Ti-8GB-Read-description/233805519514?hash=item366fe51a9a:g:AmwAAOSwh-dfx6m4</t>
         </is>
       </c>
     </row>
@@ -3393,29 +3393,29 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>New ListingGigabyte Nvidia RTX 3060 Ti EAGLE - Confirmed Order - Ships ASAP</t>
+          <t>New ListingNEW NVIDIA GEFORCE RTX 3060-TI FOUNDERS EDITION- Printed image file</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Brand New · GIGABYTE · 8 GB</t>
+          <t>Brand New · Geforce · 8 GB</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>695</v>
+        <v>450</v>
       </c>
       <c r="E93" t="n">
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="F93" t="n">
-        <v>695</v>
+        <v>457.5</v>
       </c>
       <c r="G93" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/Gigabyte-Nvidia-RTX-3060-Ti-EAGLE-Confirmed-Order-Ships-ASAP/284101390801?hash=item4225c331d1:g:SSMAAOSw~kFfx6x~</t>
+          <t>https://www.ebay.com/itm/NEW-NVIDIA-GEFORCE-RTX-3060-TI-FOUNDERS-EDITION-Printed-image-file/224261447352?hash=item3437061eb8:g:KGgAAOSwlOJfx6vb</t>
         </is>
       </c>
     </row>
@@ -3425,29 +3425,29 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>New ListingGIGABYTE GeForce RTX 3060 Ti GAMING OC PRO *Pre Sale Confirmed Order*</t>
+          <t>New ListingNvidia Geforce RTX 3060 ti Founders Edition Graphics Card 8GB GDDR6 READ</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Brand New · GIGABYTE</t>
+          <t>Brand New · Geforce · 8 GB</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>700</v>
+        <v>399</v>
       </c>
       <c r="E94" t="n">
-        <v>11.3</v>
+        <v>0</v>
       </c>
       <c r="F94" t="n">
-        <v>711.3</v>
+        <v>399</v>
       </c>
       <c r="G94" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/GIGABYTE-GeForce-RTX-3060-Ti-GAMING-OC-PRO-Pre-Sale-Confirmed-Order/124468295226?hash=item1cfae3763a:g:DSYAAOSw-R9fx60r</t>
+          <t>https://www.ebay.com/itm/Nvidia-Geforce-RTX-3060-ti-Founders-Edition-Graphics-Card-8GB-GDDR6-READ/383839013705?hash=item595e968b49:g:~v0AAOSw3Vpfx7Fu</t>
         </is>
       </c>
     </row>
@@ -3457,7 +3457,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>New ListingNvidia Geforce Rtx 3060 Ti Founders Edition (In Hand)</t>
+          <t>New ListingGeforce RTX 3060 ti Founder Edition</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -3466,20 +3466,20 @@
         </is>
       </c>
       <c r="D95" t="n">
-        <v>715</v>
+        <v>795</v>
       </c>
       <c r="E95" t="n">
-        <v>10</v>
+        <v>10.9</v>
       </c>
       <c r="F95" t="n">
-        <v>725</v>
+        <v>805.9</v>
       </c>
       <c r="G95" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/Nvidia-Geforce-Rtx-3060-Ti-Founders-Edition-In-Hand/254796360702?hash=item3b530bebfe:g:CfIAAOSw-Rlfx6-j</t>
+          <t>https://www.ebay.com/itm/Geforce-RTX-3060-ti-Founder-Edition/303792758346?hash=item46bb759e4a:g:~FcAAOSw5Clfx6uE</t>
         </is>
       </c>
     </row>
@@ -3489,29 +3489,29 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>New ListingNEW NVIDIA GEFORCE RTX 3060-TI FOUNDERS EDITION- Printed image file</t>
+          <t>New ListingGigabyte Nvidia RTX 3060 Ti EAGLE - Confirmed Order - Ships ASAP</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Brand New · Geforce · 8 GB</t>
+          <t>Brand New · GIGABYTE · 8 GB</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>450</v>
+        <v>695</v>
       </c>
       <c r="E96" t="n">
-        <v>8.25</v>
+        <v>0</v>
       </c>
       <c r="F96" t="n">
-        <v>458.25</v>
+        <v>695</v>
       </c>
       <c r="G96" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NEW-NVIDIA-GEFORCE-RTX-3060-TI-FOUNDERS-EDITION-Printed-image-file/224261410044?hash=item3437058cfc:g:KGgAAOSwlOJfx6vb</t>
+          <t>https://www.ebay.com/itm/Gigabyte-Nvidia-RTX-3060-Ti-EAGLE-Confirmed-Order-Ships-ASAP/284101390801?hash=item4225c331d1:g:SSMAAOSw~kFfx6x~</t>
         </is>
       </c>
     </row>
@@ -3521,29 +3521,29 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card  *IN HAND*</t>
+          <t>New ListingGIGABYTE GeForce RTX 3060 Ti GAMING OC PRO *Pre Sale Confirmed Order*</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Brand New · Geforce · 8 GB</t>
+          <t>Brand New · GIGABYTE</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>749.99</v>
+        <v>700</v>
       </c>
       <c r="E97" t="n">
-        <v>0</v>
+        <v>11.3</v>
       </c>
       <c r="F97" t="n">
-        <v>749.99</v>
+        <v>711.3</v>
       </c>
       <c r="G97" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card-IN-HAND/224261383874?hash=item34370526c2:g:LeQAAOSwsHhfx6kq</t>
+          <t>https://www.ebay.com/itm/GIGABYTE-GeForce-RTX-3060-Ti-GAMING-OC-PRO-Pre-Sale-Confirmed-Order/124468295226?hash=item1cfae3763a:g:DSYAAOSw-R9fx60r</t>
         </is>
       </c>
     </row>
@@ -3553,29 +3553,29 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB (Read description)</t>
+          <t>New ListingNvidia Geforce Rtx 3060 Ti Founders Edition (In Hand)</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Brand New · NVIDIA · 8 GB</t>
+          <t>Brand New · Geforce · 8 GB</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>399.99</v>
+        <v>715</v>
       </c>
       <c r="E98" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F98" t="n">
-        <v>404.99</v>
+        <v>725</v>
       </c>
       <c r="G98" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-Read-description/233805523408?hash=item366fe529d0:g:3v4AAOSw0dVfx6oN</t>
+          <t>https://www.ebay.com/itm/Nvidia-Geforce-Rtx-3060-Ti-Founders-Edition-In-Hand/254796360702?hash=item3b530bebfe:g:CfIAAOSw-Rlfx6-j</t>
         </is>
       </c>
     </row>
@@ -3585,29 +3585,29 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>New ListingNvidia RTX 3060 Ti Gigabyte AORUS- Confirmed - Fast Shipping</t>
+          <t>New ListingNEW NVIDIA GEFORCE RTX 3060-TI FOUNDERS EDITION- Printed image file</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Brand New · GIGABYTE · 8 GB</t>
+          <t>Brand New · Geforce · 8 GB</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>799</v>
+        <v>450</v>
       </c>
       <c r="E99" t="n">
-        <v>0</v>
+        <v>8.25</v>
       </c>
       <c r="F99" t="n">
-        <v>799</v>
+        <v>458.25</v>
       </c>
       <c r="G99" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/Nvidia-RTX-3060-Ti-Gigabyte-AORUS-Confirmed-Fast-Shipping/154223472146?hash=item23e86f6e12:g:mAwAAOSwX1xfx6R0</t>
+          <t>https://www.ebay.com/itm/NEW-NVIDIA-GEFORCE-RTX-3060-TI-FOUNDERS-EDITION-Printed-image-file/224261410044?hash=item3437058cfc:g:KGgAAOSwlOJfx6vb</t>
         </is>
       </c>
     </row>
@@ -3617,7 +3617,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card  *IN HAND*</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -3626,20 +3626,20 @@
         </is>
       </c>
       <c r="D100" t="n">
-        <v>630</v>
+        <v>749.99</v>
       </c>
       <c r="E100" t="n">
         <v>0</v>
       </c>
       <c r="F100" t="n">
-        <v>630</v>
+        <v>749.99</v>
       </c>
       <c r="G100" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card/363204410971?hash=item5490ab7e5b:g:eiYAAOSwj9Bfx513</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card-IN-HAND/224261383874?hash=item34370526c2:g:LeQAAOSwsHhfx6kq</t>
         </is>
       </c>
     </row>
@@ -3649,29 +3649,29 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>New ListingNvidia Geforce RTX 3060 ti Founders Edition Graphics Card 8GB GDDR6 PREORDER</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB (Read description)</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Brand New · Geforce · 8 GB</t>
+          <t>Brand New · NVIDIA · 8 GB</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>629.99</v>
+        <v>399.99</v>
       </c>
       <c r="E101" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F101" t="n">
-        <v>629.99</v>
+        <v>404.99</v>
       </c>
       <c r="G101" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/Nvidia-Geforce-RTX-3060-ti-Founders-Edition-Graphics-Card-8GB-GDDR6-PREORDER/264960899151?hash=item3db0e6784f:g:qygAAOSwQW9fx12k</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-Read-description/233805523408?hash=item366fe529d0:g:3v4AAOSw0dVfx6oN</t>
         </is>
       </c>
     </row>
@@ -3681,29 +3681,29 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card</t>
+          <t>New ListingNvidia RTX 3060 Ti Gigabyte AORUS- Confirmed - Fast Shipping</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Brand New · Geforce · 8 GB</t>
+          <t>Brand New · GIGABYTE · 8 GB</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>629.99</v>
+        <v>799</v>
       </c>
       <c r="E102" t="n">
-        <v>19.99</v>
+        <v>0</v>
       </c>
       <c r="F102" t="n">
-        <v>649.98</v>
+        <v>799</v>
       </c>
       <c r="G102" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card/363204105571?hash=item5490a6d563:g:fLAAAOSw1GBfxzik</t>
+          <t>https://www.ebay.com/itm/Nvidia-RTX-3060-Ti-Gigabyte-AORUS-Confirmed-Fast-Shipping/154223472146?hash=item23e86f6e12:g:mAwAAOSwX1xfx6R0</t>
         </is>
       </c>
     </row>
@@ -3713,29 +3713,29 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>New ListingEVGA GEFORCE RTX 3060 TI XC 8GB GDDR6 METAL BACKPLATE(PRE-ORDER)</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Brand New · EVGA · 8 GB</t>
+          <t>Brand New · Geforce · 8 GB</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>530</v>
+        <v>630</v>
       </c>
       <c r="E103" t="n">
-        <v>13.59</v>
+        <v>0</v>
       </c>
       <c r="F103" t="n">
-        <v>543.59</v>
+        <v>630</v>
       </c>
       <c r="G103" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/EVGA-GEFORCE-RTX-3060-TI-XC-8GB-GDDR6-METAL-BACKPLATE-PRE-ORDER/224260484064?hash=item3436f76be0:g:PxwAAOSwdo5fxo~~</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card/363204410971?hash=item5490ab7e5b:g:eiYAAOSwj9Bfx513</t>
         </is>
       </c>
     </row>
@@ -3745,29 +3745,29 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti Image only</t>
+          <t>New ListingNvidia Geforce RTX 3060 ti Founders Edition Graphics Card 8GB GDDR6 PREORDER</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Brand New · Geforce</t>
+          <t>Brand New · Geforce · 8 GB</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>500</v>
+        <v>629.99</v>
       </c>
       <c r="E104" t="n">
-        <v>9.9</v>
+        <v>0</v>
       </c>
       <c r="F104" t="n">
-        <v>509.9</v>
+        <v>629.99</v>
       </c>
       <c r="G104" s="2" t="n">
         <v>44167</v>
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-Image-only/284100902484?hash=item4225bbbe54:g:hlMAAOSwLndfxzNB</t>
+          <t>https://www.ebay.com/itm/Nvidia-Geforce-RTX-3060-ti-Founders-Edition-Graphics-Card-8GB-GDDR6-PREORDER/264960899151?hash=item3db0e6784f:g:qygAAOSwQW9fx12k</t>
         </is>
       </c>
     </row>
@@ -3786,20 +3786,20 @@
         </is>
       </c>
       <c r="D105" t="n">
-        <v>599.99</v>
+        <v>629.99</v>
       </c>
       <c r="E105" t="n">
         <v>19.99</v>
       </c>
       <c r="F105" t="n">
-        <v>619.98</v>
+        <v>649.98</v>
       </c>
       <c r="G105" s="2" t="n">
-        <v>44166</v>
+        <v>44167</v>
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card/363204044025?hash=item5490a5e4f9:g:fLAAAOSw1GBfxzik</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card/363204105571?hash=item5490a6d563:g:fLAAAOSw1GBfxzik</t>
         </is>
       </c>
     </row>
@@ -3809,29 +3809,29 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Nvidia Geforce RTX 3060 ti Founders Edition Graphics Card 8GB GDDR6 PREORDER</t>
+          <t>New ListingEVGA GEFORCE RTX 3060 TI XC 8GB GDDR6 METAL BACKPLATE(PRE-ORDER)</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Brand New · Geforce · 8 GB</t>
+          <t>Brand New · EVGA · 8 GB</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>700</v>
+        <v>530</v>
       </c>
       <c r="E106" t="n">
-        <v>11.3</v>
+        <v>13.59</v>
       </c>
       <c r="F106" t="n">
-        <v>711.3</v>
+        <v>543.59</v>
       </c>
       <c r="G106" s="2" t="n">
-        <v>44166</v>
+        <v>44167</v>
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/Nvidia-Geforce-RTX-3060-ti-Founders-Edition-Graphics-Card-8GB-GDDR6-PREORDER/133593780253?hash=item1f1acf501d:g:o3UAAOSwGLVfxm4s</t>
+          <t>https://www.ebay.com/itm/EVGA-GEFORCE-RTX-3060-TI-XC-8GB-GDDR6-METAL-BACKPLATE-PRE-ORDER/224260484064?hash=item3436f76be0:g:PxwAAOSwdo5fxo~~</t>
         </is>
       </c>
     </row>
@@ -3841,71 +3841,71 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>EVGA GEFORCE RTX 3060 TI XC 8GB GDDR6 METAL BACKPLATE(PRE-ORDER)</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti Image only</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Brand New · EVGA · 8 GB</t>
+          <t>Brand New · Geforce</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>530</v>
+        <v>500</v>
       </c>
       <c r="E107" t="n">
-        <v>13.59</v>
+        <v>9.9</v>
       </c>
       <c r="F107" t="n">
-        <v>543.59</v>
+        <v>509.9</v>
       </c>
       <c r="G107" s="2" t="n">
-        <v>44166</v>
+        <v>44167</v>
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/EVGA-GEFORCE-RTX-3060-TI-XC-8GB-GDDR6-METAL-BACKPLATE-PRE-ORDER/224260063237?hash=item3436f10005:g:PxwAAOSwdo5fxo~~</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-Image-only/284100902484?hash=item4225bbbe54:g:hlMAAOSwLndfxzNB</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
-        <v>212</v>
+        <v>106</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA RTX 3060 Ti GIGABYTE EAGLE OC 8GB IN HAND READY TO SHIP</t>
+          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Brand New · GIGABYTE</t>
+          <t>Brand New · Geforce · 8 GB</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>650</v>
+        <v>599.99</v>
       </c>
       <c r="E108" t="n">
-        <v>10.9</v>
+        <v>19.99</v>
       </c>
       <c r="F108" t="n">
-        <v>660.9</v>
+        <v>619.98</v>
       </c>
       <c r="G108" s="2" t="n">
-        <v>44167</v>
+        <v>44166</v>
       </c>
       <c r="H108" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-RTX-3060-Ti-GIGABYTE-EAGLE-OC-8GB-IN-HAND-READY-TO-SHIP/333811666219?hash=item4db8b9cd2b:g:tpEAAOSwbLxfyADU</t>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card/363204044025?hash=item5490a5e4f9:g:fLAAAOSw1GBfxzik</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
-        <v>213</v>
+        <v>107</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 TI Founders Edition IN HAND!!!! Limited Stock BUY NOW!!!</t>
+          <t>Nvidia Geforce RTX 3060 ti Founders Edition Graphics Card 8GB GDDR6 PREORDER</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -3914,58 +3914,58 @@
         </is>
       </c>
       <c r="D109" t="n">
-        <v>450</v>
+        <v>700</v>
       </c>
       <c r="E109" t="n">
-        <v>0</v>
+        <v>11.3</v>
       </c>
       <c r="F109" t="n">
-        <v>450</v>
+        <v>711.3</v>
       </c>
       <c r="G109" s="2" t="n">
-        <v>44167</v>
+        <v>44166</v>
       </c>
       <c r="H109" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-TI-Founders-Edition-IN-HAND-Limited-Stock-BUY-NOW/203206293280?hash=item2f5009f720:g:e7MAAOSwr15fx~hb</t>
+          <t>https://www.ebay.com/itm/Nvidia-Geforce-RTX-3060-ti-Founders-Edition-Graphics-Card-8GB-GDDR6-PREORDER/133593780253?hash=item1f1acf501d:g:o3UAAOSwGLVfxm4s</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
-        <v>214</v>
+        <v>108</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>New ListingNVIDIA GeForce RTX 3060 Ti 8GB GDDR6PCI Express 4.0 Graphics Card</t>
+          <t>EVGA GEFORCE RTX 3060 TI XC 8GB GDDR6 METAL BACKPLATE(PRE-ORDER)</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Brand New · Geforce · 8 GB</t>
+          <t>Brand New · EVGA · 8 GB</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>399.99</v>
+        <v>530</v>
       </c>
       <c r="E110" t="n">
-        <v>0</v>
+        <v>13.59</v>
       </c>
       <c r="F110" t="n">
-        <v>399.99</v>
+        <v>543.59</v>
       </c>
       <c r="G110" s="2" t="n">
-        <v>44167</v>
+        <v>44166</v>
       </c>
       <c r="H110" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-3060-Ti-8GB-GDDR6PCI-Express-4-0-Graphics-Card/313326954368?hash=item48f3bde780:g:~wwAAOSww5hfx9YC</t>
+          <t>https://www.ebay.com/itm/EVGA-GEFORCE-RTX-3060-TI-XC-8GB-GDDR6-METAL-BACKPLATE-PRE-ORDER/224260063237?hash=item3436f10005:g:PxwAAOSwdo5fxo~~</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
-        <v>250</v>
+        <v>147</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
@@ -3997,7 +3997,7 @@
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
-        <v>310</v>
+        <v>207</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
@@ -4029,7 +4029,7 @@
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
-        <v>317</v>
+        <v>214</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>

</xml_diff>